<commit_message>
test for unique column labels
</commit_message>
<xml_diff>
--- a/test/general.xlsx
+++ b/test/general.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noronha/.julia/v0.6/XLSX/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA6A21-28DA-1647-A85B-30F73601BA2F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -22,8 +23,9 @@
     <sheet name="table6" sheetId="8" r:id="rId8"/>
     <sheet name="table7" sheetId="9" r:id="rId9"/>
     <sheet name="lookup" sheetId="10" r:id="rId10"/>
+    <sheet name="header_error" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>text</t>
   </si>
@@ -166,11 +168,26 @@
   <si>
     <t>name3</t>
   </si>
+  <si>
+    <t>COLUMN_A</t>
+  </si>
+  <si>
+    <t>COLUMN_B</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>there</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -485,10 +502,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -551,10 +568,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -663,8 +680,56 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122C239-B27E-4F47-96FD-DE9E78741957}">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -722,7 +787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="E12:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -763,7 +828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -976,7 +1041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1028,7 +1093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1042,7 +1107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1087,7 +1152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1137,7 +1202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>